<commit_message>
some front end on settings page
</commit_message>
<xml_diff>
--- a/GUI/Vacations_History.xlsx
+++ b/GUI/Vacations_History.xlsx
@@ -470,7 +470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC71"/>
+  <dimension ref="A1:AC75"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10802,6 +10802,586 @@
         </is>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>2024-06-19</t>
+        </is>
+      </c>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>الأربعاء</t>
+        </is>
+      </c>
+      <c r="D72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="E72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="F72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="H72" s="7" t="inlineStr">
+        <is>
+          <t>إمتداد</t>
+        </is>
+      </c>
+      <c r="I72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="J72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="K72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="L72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="M72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="N72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="O72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="P72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Q72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="R72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="S72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="T72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="U72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="V72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="W72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="X72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Y72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Z72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AA72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AB72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AC72" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
+        <is>
+          <t>2024-06-20</t>
+        </is>
+      </c>
+      <c r="C73" s="4" t="inlineStr">
+        <is>
+          <t>الخميس</t>
+        </is>
+      </c>
+      <c r="D73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="E73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="F73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="G73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="H73" s="7" t="inlineStr">
+        <is>
+          <t>إمتداد</t>
+        </is>
+      </c>
+      <c r="I73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="J73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="K73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="L73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="M73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="N73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="O73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="P73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Q73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="R73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="S73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="T73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="U73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="V73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="W73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="X73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Y73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Z73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AA73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AB73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AC73" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>2024-06-21</t>
+        </is>
+      </c>
+      <c r="C74" s="4" t="inlineStr">
+        <is>
+          <t>الجمعة</t>
+        </is>
+      </c>
+      <c r="D74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="E74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="F74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="H74" s="7" t="inlineStr">
+        <is>
+          <t>إمتداد</t>
+        </is>
+      </c>
+      <c r="I74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="J74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="K74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="L74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="M74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="N74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="O74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="P74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Q74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="R74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="S74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="T74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="U74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="V74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="W74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="X74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Y74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Z74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AA74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AB74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AC74" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
+        <is>
+          <t>2024-06-22</t>
+        </is>
+      </c>
+      <c r="C75" s="4" t="inlineStr">
+        <is>
+          <t>السبت</t>
+        </is>
+      </c>
+      <c r="D75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="E75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="F75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="G75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="H75" s="7" t="inlineStr">
+        <is>
+          <t>إمتداد</t>
+        </is>
+      </c>
+      <c r="I75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="J75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="K75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="L75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="M75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="N75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="O75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="P75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Q75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="R75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="S75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="T75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="U75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="V75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="W75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="X75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Y75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="Z75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AA75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AB75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+      <c r="AC75" s="5" t="inlineStr">
+        <is>
+          <t>موجود</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>